<commit_message>
Added requirements phase report
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tritet\Desktop\VVSS\repo\VVSS\Docs\Lab01\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="156" windowWidth="14160" windowHeight="8268" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1050" windowWidth="14160" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
     <sheet name="Architect. Design Phase Defects" sheetId="6" r:id="rId2"/>
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -27,9 +32,6 @@
     <t>Reviewer Name:</t>
   </si>
   <si>
-    <t>do not print this form</t>
-  </si>
-  <si>
     <t>Crt. No.</t>
   </si>
   <si>
@@ -51,24 +53,12 @@
     <t xml:space="preserve">Author Name: </t>
   </si>
   <si>
-    <t>Popescu Ionel</t>
-  </si>
-  <si>
-    <t>Georgescu Anca</t>
-  </si>
-  <si>
-    <t>Firicescu George</t>
-  </si>
-  <si>
     <t>Requirements Document</t>
   </si>
   <si>
     <t>Architectural Design Document</t>
   </si>
   <si>
-    <t>Coding Document</t>
-  </si>
-  <si>
     <t>Review Form. Coding Defects</t>
   </si>
   <si>
@@ -76,12 +66,39 @@
   </si>
   <si>
     <t>Review Form. Requirements Defects</t>
+  </si>
+  <si>
+    <t>10.03.2019</t>
+  </si>
+  <si>
+    <t>Tritean Tudor-Adrian</t>
+  </si>
+  <si>
+    <t>Coding document</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>R03</t>
+  </si>
+  <si>
+    <t>The type of the report is not defined(pdf,etc.)</t>
+  </si>
+  <si>
+    <t>Authentication is not even mentioned</t>
+  </si>
+  <si>
+    <t>Properties of a user are defined while describing a functionality</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -230,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -266,19 +283,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -299,6 +304,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -347,7 +355,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -382,7 +390,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -596,52 +604,50 @@
   </sheetPr>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.3125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="22"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>8</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="24"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -649,54 +655,68 @@
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="E7" s="20"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -705,7 +725,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -714,7 +734,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -723,7 +743,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -732,7 +752,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -741,7 +761,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -750,7 +770,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -759,7 +779,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -768,7 +788,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -777,7 +797,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -786,7 +806,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="16"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -795,7 +815,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="16"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -804,7 +824,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="16"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -813,15 +833,17 @@
       <c r="D25" s="3"/>
       <c r="E25" s="16"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -843,52 +865,50 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.3125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="23"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D4" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="21"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="25"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>9</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="24"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -896,28 +916,30 @@
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="E7" s="20"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -925,7 +947,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -934,7 +956,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -943,7 +965,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -952,7 +974,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -961,7 +983,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -970,7 +992,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -979,7 +1001,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -988,7 +1010,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -997,7 +1019,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1006,7 +1028,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1015,7 +1037,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1024,7 +1046,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1033,7 +1055,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1042,7 +1064,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1051,7 +1073,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1060,7 +1082,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1069,15 +1091,17 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C28" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28" s="13"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1099,53 +1123,51 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.3125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.89453125" style="6"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="22"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="26"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="28"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E5" s="24"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1153,28 +1175,30 @@
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="E7" s="20"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1182,7 +1206,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1191,7 +1215,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1200,7 +1224,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1209,7 +1233,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1218,7 +1242,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1227,7 +1251,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1236,7 +1260,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1245,7 +1269,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1254,7 +1278,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1263,7 +1287,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1272,7 +1296,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1281,7 +1305,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1290,7 +1314,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1299,7 +1323,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1308,7 +1332,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1317,7 +1341,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1326,7 +1350,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1335,7 +1359,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1344,7 +1368,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1353,7 +1377,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1362,15 +1386,17 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D32" s="13"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1383,4 +1409,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <msg_Klassifizierung xmlns="1dd69248-66f9-453d-8211-ae5ae34a4b30">internal</msg_Klassifizierung>
+    <msg_Status xmlns="1dd69248-66f9-453d-8211-ae5ae34a4b30">draft</msg_Status>
+    <msg_Firma xmlns="1dd69248-66f9-453d-8211-ae5ae34a4b30">msg</msg_Firma>
+    <msg_Version xmlns="1dd69248-66f9-453d-8211-ae5ae34a4b30">0.1</msg_Version>
+    <msg_Manager xmlns="1dd69248-66f9-453d-8211-ae5ae34a4b30">[Dokumentverantwortlicher]</msg_Manager>
+    <msg_Dokumententyp xmlns="1dd69248-66f9-453d-8211-ae5ae34a4b30">Schriftwechsel (allgemein)</msg_Dokumententyp>
+    <msg_gueltig_ab xmlns="1dd69248-66f9-453d-8211-ae5ae34a4b30">2019-03-10T12:00:00+00:00</msg_gueltig_ab>
+    <msg_gueltig_bis xmlns="1dd69248-66f9-453d-8211-ae5ae34a4b30">2025-12-31T12:00:00+00:00</msg_gueltig_bis>
+    <msg_Kommentar xmlns="1dd69248-66f9-453d-8211-ae5ae34a4b30">Neues Dokument erstellt.</msg_Kommentar>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA9E225E-5E00-4B8D-BBCB-939932F35D10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1dd69248-66f9-453d-8211-ae5ae34a4b30"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added architectural design phase report
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1050" windowWidth="14160" windowHeight="8265"/>
+    <workbookView xWindow="0" yWindow="1500" windowWidth="14160" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -93,6 +93,24 @@
   </si>
   <si>
     <t>Properties of a user are defined while describing a functionality</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>Architecture diagram is chaotic and not comprehensive</t>
+  </si>
+  <si>
+    <t>The architecure does not define the entities used for the application</t>
+  </si>
+  <si>
+    <t>Useless packages/classes and layering issues are present</t>
   </si>
 </sst>
 </file>
@@ -283,16 +301,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -605,7 +623,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,10 +660,10 @@
       <c r="C5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
@@ -685,7 +703,9 @@
       <c r="C10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>21</v>
       </c>
@@ -698,7 +718,9 @@
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
       <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
@@ -711,7 +733,9 @@
       <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
       <c r="E12" s="2" t="s">
         <v>23</v>
       </c>
@@ -866,7 +890,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,19 +918,19 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
@@ -939,31 +963,49 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
@@ -1153,19 +1195,19 @@
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="22"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>

</xml_diff>

<commit_message>
Added program coding phase report
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1500" windowWidth="14160" windowHeight="8265"/>
+    <workbookView xWindow="0" yWindow="1950" windowWidth="14160" windowHeight="8265" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -111,6 +111,33 @@
   </si>
   <si>
     <t>Useless packages/classes and layering issues are present</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>File Repos</t>
+  </si>
+  <si>
+    <t>Input data is not obtained due to incorrect input files paths</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Duration is a time and it is declared as a date for e.g. but there are so many things to take into account here regarding variable naming, redundant null initializations and so on and so forth</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>Architectural decisions mainly, which consist of bad packaging and layering, wrong location for many classes and/or interfaces, for e.g. the repositories which are in a model package plus some weird output messages decisions and so on</t>
+  </si>
+  <si>
+    <t>Everywhere</t>
   </si>
 </sst>
 </file>
@@ -622,7 +649,7 @@
   </sheetPr>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -1165,8 +1192,8 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,31 +1267,49 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3">

</xml_diff>

<commit_message>
Fix some things for the report
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1950" windowWidth="14160" windowHeight="8265" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="14160" windowHeight="8265" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -116,18 +116,12 @@
     <t>C06</t>
   </si>
   <si>
-    <t>File Repos</t>
-  </si>
-  <si>
     <t>Input data is not obtained due to incorrect input files paths</t>
   </si>
   <si>
     <t>C12</t>
   </si>
   <si>
-    <t>Activity</t>
-  </si>
-  <si>
     <t>Duration is a time and it is declared as a date for e.g. but there are so many things to take into account here regarding variable naming, redundant null initializations and so on and so forth</t>
   </si>
   <si>
@@ -138,6 +132,15 @@
   </si>
   <si>
     <t>Everywhere</t>
+  </si>
+  <si>
+    <t>Diagram</t>
+  </si>
+  <si>
+    <t>File Repos, lines 18-19</t>
+  </si>
+  <si>
+    <t>Activity, line 12</t>
   </si>
 </sst>
 </file>
@@ -917,7 +920,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,8 +1000,8 @@
       <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="2">
-        <v>1</v>
+      <c r="D10" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>27</v>
@@ -1012,8 +1015,8 @@
       <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="2">
-        <v>1</v>
+      <c r="D11" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>29</v>
@@ -1027,8 +1030,8 @@
       <c r="C12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="1">
-        <v>1</v>
+      <c r="D12" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>28</v>
@@ -1193,7 +1196,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,10 +1278,10 @@
         <v>30</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1287,13 +1290,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1302,13 +1305,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated a description in the program coding phase
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="14160" windowHeight="8265" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2850" windowWidth="14160" windowHeight="8265" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -119,12 +119,6 @@
     <t>Input data is not obtained due to incorrect input files paths</t>
   </si>
   <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>Duration is a time and it is declared as a date for e.g. but there are so many things to take into account here regarding variable naming, redundant null initializations and so on and so forth</t>
-  </si>
-  <si>
     <t>C01</t>
   </si>
   <si>
@@ -141,6 +135,12 @@
   </si>
   <si>
     <t>Activity, line 12</t>
+  </si>
+  <si>
+    <t>C09</t>
+  </si>
+  <si>
+    <t>As a class field, it is named in some way, but then, in the constructor it is named differently, suggesting another purpose, for e.g. in the Activity class, we have a Date field called duration which does not suggest a Date, but a number of hours, days and so on, and in the constructor it is actually called end which might suggest that it is indeed a date (an end-date)</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1001,7 @@
         <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>27</v>
@@ -1016,7 +1016,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>29</v>
@@ -1031,7 +1031,7 @@
         <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>28</v>
@@ -1196,7 +1196,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,25 +1278,25 @@
         <v>30</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1305,13 +1305,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>